<commit_message>
Updated file by pankaj for groupb
</commit_message>
<xml_diff>
--- a/DevOps_Trainee.xlsx
+++ b/DevOps_Trainee.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Suyash\DevOps\Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\panparab\CG_DevOps_Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8870D3F5-65D4-412C-B9CD-5CD77F15DAFD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9140" windowHeight="2180"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>DevOps Trainee</t>
   </si>
@@ -51,12 +52,36 @@
   </si>
   <si>
     <t>Group-C</t>
+  </si>
+  <si>
+    <t>pankaj</t>
+  </si>
+  <si>
+    <t>suraj</t>
+  </si>
+  <si>
+    <t>vaibhav</t>
+  </si>
+  <si>
+    <t>cyril</t>
+  </si>
+  <si>
+    <t>chetan</t>
+  </si>
+  <si>
+    <t>unix</t>
+  </si>
+  <si>
+    <t>wintel</t>
+  </si>
+  <si>
+    <t>automation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -549,14 +574,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:G17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C1" s="9" t="s">
@@ -633,46 +661,76 @@
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3">
+        <v>13309</v>
+      </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13310</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3">
+        <v>13312</v>
+      </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="3">
+        <v>13313</v>
+      </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="3">
+        <v>13314</v>
+      </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C13" s="2" t="s">

</xml_diff>